<commit_message>
Identical to tb-ucl analyses branch
</commit_message>
<xml_diff>
--- a/project/databook-belarus-template.xlsx
+++ b/project/databook-belarus-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="-2060" yWindow="100" windowWidth="25600" windowHeight="15520" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -635,7 +635,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -663,16 +663,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -686,6 +693,9 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -699,6 +709,9 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6634,8 +6647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6711,12 +6724,15 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="str">
         <f t="shared" ref="C2:C7" si="0">IF(SUMPRODUCT(--(E2:T2&lt;&gt;""))=0,0.2,"N.A.")</f>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -6727,12 +6743,15 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="str">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -6743,12 +6762,15 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -6759,12 +6781,15 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -6775,12 +6800,15 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -6791,12 +6819,15 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -6866,12 +6897,15 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="str">
         <f t="shared" ref="C10:C15" si="1">IF(SUMPRODUCT(--(E10:T10&lt;&gt;""))=0,0.15,"N.A.")</f>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -6882,12 +6916,15 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -6898,12 +6935,15 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -6914,12 +6954,15 @@
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -6930,12 +6973,15 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -6946,12 +6992,15 @@
       <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -7021,12 +7070,15 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="str">
         <f t="shared" ref="C18:C23" si="2">IF(SUMPRODUCT(--(E18:T18&lt;&gt;""))=0,0.15,"N.A.")</f>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -7037,12 +7089,15 @@
       <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="str">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -7053,12 +7108,15 @@
       <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="str">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -7069,12 +7127,15 @@
       <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="str">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -7085,12 +7146,15 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="str">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -7101,12 +7165,15 @@
       <c r="B23" t="s">
         <v>10</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="str">
         <f t="shared" si="2"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -7176,12 +7243,15 @@
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="str">
         <f t="shared" ref="C26:C31" si="3">IF(SUMPRODUCT(--(E26:T26&lt;&gt;""))=0,0.2,"N.A.")</f>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:20">
@@ -7192,12 +7262,15 @@
       <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="str">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:20">
@@ -7208,12 +7281,15 @@
       <c r="B28" t="s">
         <v>10</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="str">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:20">
@@ -7224,12 +7300,15 @@
       <c r="B29" t="s">
         <v>10</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="str">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:20">
@@ -7240,12 +7319,15 @@
       <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="str">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:20">
@@ -7256,12 +7338,15 @@
       <c r="B31" t="s">
         <v>10</v>
       </c>
-      <c r="C31">
+      <c r="C31" t="str">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:20">
@@ -7331,12 +7416,15 @@
       <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="str">
         <f t="shared" ref="C34:C39" si="4">IF(SUMPRODUCT(--(E34:T34&lt;&gt;""))=0,0.15,"N.A.")</f>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:20">
@@ -7347,12 +7435,15 @@
       <c r="B35" t="s">
         <v>10</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="str">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:20">
@@ -7363,12 +7454,15 @@
       <c r="B36" t="s">
         <v>10</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="str">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:20">
@@ -7379,12 +7473,15 @@
       <c r="B37" t="s">
         <v>10</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="str">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:20">
@@ -7395,12 +7492,15 @@
       <c r="B38" t="s">
         <v>10</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="str">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:20">
@@ -7411,12 +7511,15 @@
       <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="str">
         <f t="shared" si="4"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:20">
@@ -7486,12 +7589,15 @@
       <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="str">
         <f t="shared" ref="C42:C47" si="5">IF(SUMPRODUCT(--(E42:T42&lt;&gt;""))=0,0.15,"N.A.")</f>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -7502,12 +7608,15 @@
       <c r="B43" t="s">
         <v>10</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="str">
         <f t="shared" si="5"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -7518,12 +7627,15 @@
       <c r="B44" t="s">
         <v>10</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="str">
         <f t="shared" si="5"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -7534,12 +7646,15 @@
       <c r="B45" t="s">
         <v>10</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="str">
         <f t="shared" si="5"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -7550,12 +7665,15 @@
       <c r="B46" t="s">
         <v>10</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="str">
         <f t="shared" si="5"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -7566,12 +7684,15 @@
       <c r="B47" t="s">
         <v>10</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="str">
         <f t="shared" si="5"/>
-        <v>0.15</v>
+        <v>N.A.</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -8390,8 +8511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8475,7 +8596,7 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -8494,7 +8615,7 @@
         <v>12</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -8513,7 +8634,7 @@
         <v>12</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -8532,7 +8653,7 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -8543,12 +8664,15 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -8559,12 +8683,15 @@
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:20">
@@ -8642,7 +8769,7 @@
         <v>12</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -8661,7 +8788,7 @@
         <v>12</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -8680,7 +8807,7 @@
         <v>12</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -8699,7 +8826,7 @@
         <v>12</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -8710,12 +8837,15 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -8726,12 +8856,15 @@
       <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:20">
@@ -8801,12 +8934,15 @@
       <c r="B18" t="s">
         <v>10</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="str">
         <f t="shared" ref="C18:C23" si="2">IF(SUMPRODUCT(--(E18:T18&lt;&gt;""))=0,0.7,"N.A.")</f>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:20">
@@ -8817,12 +8953,15 @@
       <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="str">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:20">
@@ -8833,12 +8972,15 @@
       <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="str">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:20">
@@ -8849,12 +8991,15 @@
       <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="str">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:20">
@@ -8865,12 +9010,15 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="str">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20">
@@ -8881,12 +9029,15 @@
       <c r="B23" t="s">
         <v>10</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="str">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>N.A.</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:20">
@@ -9577,12 +9728,15 @@
       <c r="B50" t="s">
         <v>10</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="str">
         <f t="shared" ref="C50:C55" si="6">IF(SUMPRODUCT(--(E50:T50&lt;&gt;""))=0,0.2,"N.A.")</f>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -9593,12 +9747,15 @@
       <c r="B51" t="s">
         <v>10</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="str">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -9609,12 +9766,15 @@
       <c r="B52" t="s">
         <v>10</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="str">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:20">
@@ -9625,12 +9785,15 @@
       <c r="B53" t="s">
         <v>10</v>
       </c>
-      <c r="C53">
+      <c r="C53" t="str">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:20">
@@ -9641,12 +9804,15 @@
       <c r="B54" t="s">
         <v>10</v>
       </c>
-      <c r="C54">
+      <c r="C54" t="str">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:20">
@@ -9657,12 +9823,15 @@
       <c r="B55" t="s">
         <v>10</v>
       </c>
-      <c r="C55">
+      <c r="C55" t="str">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:20">
@@ -9732,12 +9901,15 @@
       <c r="B58" t="s">
         <v>10</v>
       </c>
-      <c r="C58">
+      <c r="C58" t="str">
         <f t="shared" ref="C58:C63" si="7">IF(SUMPRODUCT(--(E58:T58&lt;&gt;""))=0,0.2,"N.A.")</f>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:20">
@@ -9748,12 +9920,15 @@
       <c r="B59" t="s">
         <v>10</v>
       </c>
-      <c r="C59">
+      <c r="C59" t="str">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:20">
@@ -9764,12 +9939,15 @@
       <c r="B60" t="s">
         <v>10</v>
       </c>
-      <c r="C60">
+      <c r="C60" t="str">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:20">
@@ -9780,12 +9958,15 @@
       <c r="B61" t="s">
         <v>10</v>
       </c>
-      <c r="C61">
+      <c r="C61" t="str">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:20">
@@ -9796,12 +9977,15 @@
       <c r="B62" t="s">
         <v>10</v>
       </c>
-      <c r="C62">
+      <c r="C62" t="str">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:20">
@@ -9812,12 +9996,15 @@
       <c r="B63" t="s">
         <v>10</v>
       </c>
-      <c r="C63">
+      <c r="C63" t="str">
         <f t="shared" si="7"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:20">
@@ -9887,12 +10074,15 @@
       <c r="B66" t="s">
         <v>10</v>
       </c>
-      <c r="C66">
+      <c r="C66" t="str">
         <f t="shared" ref="C66:C71" si="8">IF(SUMPRODUCT(--(E66:T66&lt;&gt;""))=0,0.2,"N.A.")</f>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D66" t="s">
         <v>12</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:20">
@@ -9903,12 +10093,15 @@
       <c r="B67" t="s">
         <v>10</v>
       </c>
-      <c r="C67">
+      <c r="C67" t="str">
         <f t="shared" si="8"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:20">
@@ -9919,12 +10112,15 @@
       <c r="B68" t="s">
         <v>10</v>
       </c>
-      <c r="C68">
+      <c r="C68" t="str">
         <f t="shared" si="8"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D68" t="s">
         <v>12</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:20">
@@ -9935,12 +10131,15 @@
       <c r="B69" t="s">
         <v>10</v>
       </c>
-      <c r="C69">
+      <c r="C69" t="str">
         <f t="shared" si="8"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D69" t="s">
         <v>12</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:20">
@@ -9951,12 +10150,15 @@
       <c r="B70" t="s">
         <v>10</v>
       </c>
-      <c r="C70">
+      <c r="C70" t="str">
         <f t="shared" si="8"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:20">
@@ -9967,12 +10169,15 @@
       <c r="B71" t="s">
         <v>10</v>
       </c>
-      <c r="C71">
+      <c r="C71" t="str">
         <f t="shared" si="8"/>
-        <v>0.2</v>
+        <v>N.A.</v>
       </c>
       <c r="D71" t="s">
         <v>12</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:20">
@@ -11684,7 +11889,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -13570,7 +13777,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14000,52 +14207,52 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>90068.800000000003</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>90068.800000000003</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>90068.800000000003</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>90068.800000000003</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>90068.800000000003</v>
       </c>
-      <c r="J10">
-        <v>102352.40000000001</v>
-      </c>
-      <c r="K10">
-        <v>102352.40000000001</v>
-      </c>
-      <c r="L10">
-        <v>102352.40000000001</v>
-      </c>
-      <c r="M10">
-        <v>102352.40000000001</v>
-      </c>
-      <c r="N10">
-        <v>102352.40000000001</v>
-      </c>
-      <c r="O10">
-        <v>111124.59999999999</v>
-      </c>
-      <c r="P10">
-        <v>111124.59999999999</v>
-      </c>
-      <c r="Q10">
-        <v>111124.59999999999</v>
-      </c>
-      <c r="R10">
-        <v>111124.59999999999</v>
-      </c>
-      <c r="S10">
-        <v>111124.59999999999</v>
-      </c>
-      <c r="T10">
+      <c r="J10" s="2">
+        <v>102352.4</v>
+      </c>
+      <c r="K10" s="2">
+        <v>102352.4</v>
+      </c>
+      <c r="L10" s="2">
+        <v>102352.4</v>
+      </c>
+      <c r="M10" s="2">
+        <v>102352.4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>102352.4</v>
+      </c>
+      <c r="O10" s="2">
+        <v>111124.6</v>
+      </c>
+      <c r="P10" s="2">
+        <v>111124.6</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>111124.6</v>
+      </c>
+      <c r="R10" s="2">
+        <v>111124.6</v>
+      </c>
+      <c r="S10" s="2">
+        <v>111124.6</v>
+      </c>
+      <c r="T10" s="2">
         <v>109426.4</v>
       </c>
     </row>
@@ -14547,7 +14754,7 @@
   <dimension ref="A1:T175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R81" sqref="R81"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14811,15 +15018,20 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="str">
         <f t="shared" ref="C10:C15" si="1">IF(SUMPRODUCT(--(E10:T10&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="P10" s="6">
+        <f>P2*0.8571429</f>
+        <v>1895.8860947942999</v>
+      </c>
+      <c r="R10" s="6">
+        <v>2768</v>
+      </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="str">
@@ -14829,15 +15041,21 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="P11" s="6">
+        <f>P3*0.1578947</f>
+        <v>589.72628344980001</v>
+      </c>
+      <c r="R11" s="6">
+        <f>R3*0.27272727</f>
+        <v>1204.2667515936962</v>
+      </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="str">
@@ -14847,15 +15065,21 @@
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="4"/>
-      <c r="R12" s="4"/>
+      <c r="P12" s="6">
+        <f>P4*0.6630765</f>
+        <v>42933.798102643195</v>
+      </c>
+      <c r="R12" s="6">
+        <f>R4*0.954744</f>
+        <v>60782.026714248001</v>
+      </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="str">
@@ -14865,15 +15089,21 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="P13" s="6">
+        <f>0.5811808*P5</f>
+        <v>7401.5076577382415</v>
+      </c>
+      <c r="R13" s="6">
+        <f>R5*0.626667</f>
+        <v>7914.276243052499</v>
+      </c>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="str">
@@ -14974,15 +15204,20 @@
       <c r="B18" t="s">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="str">
         <f t="shared" ref="C18:C23" si="2">IF(SUMPRODUCT(--(E18:T18&lt;&gt;""))=0,0,"N.A.")</f>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="P18" s="4"/>
-      <c r="R18" s="4"/>
+      <c r="P18">
+        <f>0.1428571*P2</f>
+        <v>315.98090520569991</v>
+      </c>
+      <c r="R18" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="str">
@@ -14992,15 +15227,21 @@
       <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
-      <c r="P19" s="4"/>
-      <c r="R19" s="4"/>
+      <c r="P19">
+        <f>P3*0.8421953</f>
+        <v>3145.5438606101998</v>
+      </c>
+      <c r="R19" s="6">
+        <f>R3*0.72727273</f>
+        <v>3211.3780484063041</v>
+      </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="str">
@@ -15010,15 +15251,21 @@
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20">
+      <c r="C20" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="4"/>
-      <c r="R20" s="4"/>
+      <c r="P20">
+        <f>P4*0.3369235</f>
+        <v>21815.590697356798</v>
+      </c>
+      <c r="R20" s="6">
+        <f>R4*0.045256</f>
+        <v>2881.1402857519997</v>
+      </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="str">
@@ -15028,15 +15275,21 @@
       <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="C21">
+      <c r="C21" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>N.A.</v>
       </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
-      <c r="P21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="P21">
+        <f>P5*0.4188192</f>
+        <v>5333.7851422617605</v>
+      </c>
+      <c r="R21" s="6">
+        <f>R5*0.3733333</f>
+        <v>4714.8850456947494</v>
+      </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="str">
@@ -18431,6 +18684,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -18444,7 +18698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
@@ -22736,7 +22990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>

</xml_diff>